<commit_message>
membuat fungsi tambah file
</commit_message>
<xml_diff>
--- a/upload/65bb0bdd2c295.xlsx
+++ b/upload/65bb0bdd2c295.xlsx
@@ -1,130 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tari\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03EC779-6802-48F5-9DF3-2466FB1D887C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Full" sheetId="2" r:id="rId1"/>
-    <sheet name="Amend" sheetId="6" state="hidden" r:id="rId2"/>
-    <sheet name="Action" sheetId="8" state="hidden" r:id="rId3"/>
-    <sheet name="Pending Approval" sheetId="9" state="hidden" r:id="rId4"/>
-    <sheet name="Pending at Bank" sheetId="10" state="hidden" r:id="rId5"/>
+    <sheet name="Full" sheetId="1" r:id="rId4"/>
+    <sheet name="Amend" sheetId="2" state="hidden" r:id="rId5"/>
+    <sheet name="Action" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="Pending Approval" sheetId="4" state="hidden" r:id="rId7"/>
+    <sheet name="Pending at Bank" sheetId="5" state="hidden" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="234">
+  <si>
+    <t>Test Date</t>
+  </si>
+  <si>
+    <t>PIC</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Modul</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Test Step</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>TC Web Status</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>TC Web Capture</t>
+  </si>
+  <si>
+    <t>2024-02-08</t>
+  </si>
+  <si>
+    <t>Fatur</t>
+  </si>
+  <si>
+    <t>FCC - CA - TS - SG - 001</t>
+  </si>
+  <si>
+    <t>Suki Dakara cuyttesrdytfguhij</t>
+  </si>
+  <si>
+    <t>Shipping Guarantee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click Menu </t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>1. Login application FCC as Client Admin2. Dashboard Client Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click Menu </t>
+  </si>
+  <si>
+    <t>ewrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successfully click and display </t>
+  </si>
   <si>
     <t>Not Tested</t>
   </si>
   <si>
-    <t>Modul</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>Client Admin - Trade Service</t>
-  </si>
-  <si>
-    <t>Shipping Guarantee</t>
-  </si>
-  <si>
-    <t>Shipping Guarantee - Dashboard</t>
-  </si>
-  <si>
-    <t>Shipping Guarantee - Live</t>
-  </si>
-  <si>
-    <t>Shipping Guarantee - Reject</t>
-  </si>
-  <si>
-    <t>Shipping Guarantee - Draft</t>
-  </si>
-  <si>
-    <t>Bank Admin - Middle Office</t>
-  </si>
-  <si>
-    <t>Pending Record - List of Record Shipping Guarantee Live</t>
-  </si>
-  <si>
-    <t>Pending Record - List of Record Shipping Guarantee Reject</t>
-  </si>
-  <si>
-    <t>Test Date</t>
-  </si>
-  <si>
-    <t>PIC</t>
-  </si>
-  <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
-    <t>Test Case</t>
-  </si>
-  <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>Pre-Condition</t>
-  </si>
-  <si>
-    <t>Test Step</t>
-  </si>
-  <si>
-    <t>Test Data</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>TC Web Status</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>TC Web Capture</t>
-  </si>
-  <si>
-    <t>FCC - CA - TS - SG - 001</t>
-  </si>
-  <si>
-    <t>Click Menu "Shipping Guarantee"</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>1. Login application FCC as Client Admin
-2. Dashboard Client Admin</t>
-  </si>
-  <si>
-    <t>1. Click Menu "Trade Service"
-2. Click Sub Menu "Shipping Guarantee"</t>
-  </si>
-  <si>
-    <t>Successfully click and display "Shipping Guarantee" Dashboard page</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
+    <t>2024-02-06</t>
+  </si>
+  <si>
+    <t>Tri Amin Ridho</t>
+  </si>
+  <si>
     <t>FCC - CA - TS - SG - 002</t>
+  </si>
+  <si>
+    <t>Client Admin - Trade Service OKE</t>
   </si>
   <si>
     <t>Click Button "Request Shipping Guarantee"</t>
@@ -141,7 +131,16 @@
     <t xml:space="preserve">Successfully click and display "General Details" Section in Shipping Guarantee Initiation page </t>
   </si>
   <si>
+    <t>2024-02-14</t>
+  </si>
+  <si>
     <t>FCC - CA - TS - SGL - 001</t>
+  </si>
+  <si>
+    <t>Client Admin - Trade Service xxxxxxxxxxxx baru ubah</t>
+  </si>
+  <si>
+    <t>Shipping Guarantee - Live</t>
   </si>
   <si>
     <t>Click Menu Form Section "General Details"</t>
@@ -155,6 +154,9 @@
   </si>
   <si>
     <t>FCC - CA - TS - SGL - 002</t>
+  </si>
+  <si>
+    <t>Client Admin - Trade Service</t>
   </si>
   <si>
     <t>Click Menu Form Section "Applicant and Beneficiary Details"</t>
@@ -567,6 +569,12 @@
     <t>FCC - BA - MO - PL - LRSGL - 001</t>
   </si>
   <si>
+    <t>Bank Admin - Middle Office</t>
+  </si>
+  <si>
+    <t>Pending Record - List of Record Shipping Guarantee Live</t>
+  </si>
+  <si>
     <t>Approve shipping Guarantee with Input Only Mandatory Field by User Bank Admin</t>
   </si>
   <si>
@@ -602,6 +610,9 @@
   </si>
   <si>
     <t>FCC - CA - TS - SGR - 001</t>
+  </si>
+  <si>
+    <t>Shipping Guarantee - Reject</t>
   </si>
   <si>
     <t>Create shipping Guarantee with Input Only Mandatory Field For Reject from Another User Client Admin</t>
@@ -693,6 +704,9 @@
     <t>FCC - BA - MO - PL - LRSGR - 001</t>
   </si>
   <si>
+    <t>Pending Record - List of Record Shipping Guarantee Reject</t>
+  </si>
+  <si>
     <t>Reject shipping Guarantee with Input Mandatory Field by User Bank Admin</t>
   </si>
   <si>
@@ -719,6 +733,9 @@
   </si>
   <si>
     <t>FCC - CA - TS - SGD - 001</t>
+  </si>
+  <si>
+    <t>Shipping Guarantee - Draft</t>
   </si>
   <si>
     <t>Create Shipping Guarantee with Input Only Mandatory Field</t>
@@ -772,7 +789,14 @@
 - The Shipping Guarantee appear at Dashboard with Status Draft</t>
   </si>
   <si>
+    <t>Shipping Guarantee - Dashboard</t>
+  </si>
+  <si>
     <t>Click Status Tab "Live" at Shipping Guarantee Dashboard page</t>
+  </si>
+  <si>
+    <t>1. Login application FCC as Client Admin
+2. Dashboard Client Admin</t>
   </si>
   <si>
     <t>1. Click Menu "Trade Service"
@@ -865,37 +889,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -922,7 +955,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -935,9 +970,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -954,61 +987,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -1062,131 +1087,160 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1197,73 +1251,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="15.75" defaultColWidth="12.6640625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="11" max="12" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="4.33203125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20.44140625" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20.44140625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="25.33203125" customWidth="true" style="0"/>
+    <col min="9" max="9" width="27.6640625" customWidth="true" style="0"/>
+    <col min="11" max="11" width="25.77734375" customWidth="true" style="0"/>
+    <col min="12" max="12" width="25.77734375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -1277,1974 +1332,2003 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:26">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:26">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="I32" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>10</v>
+        <v>158</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>11</v>
+        <v>188</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>11</v>
+        <v>188</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="10" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="10" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="10" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="2" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I49" s="2" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="2" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="2" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="2" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="2" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M52" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L52" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="1" sqref="G2:G52">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="1" sqref="L2:L52">
       <formula1>"Not Tested,Passed,Failed,On Testing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G52" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"Positive,Negative"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M52" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="1" sqref="M2:M52">
       <formula1>"None,Showstopper,Blocker,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="15.75" defaultColWidth="12.6640625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="4.44140625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="6.6640625" customWidth="true" style="0"/>
+    <col min="4" max="4" width="16.33203125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -3258,89 +3342,100 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="15.75" defaultColWidth="12.6640625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="33.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" customWidth="true" style="0"/>
+    <col min="2" max="2" width="5.88671875" customWidth="true" style="0"/>
+    <col min="6" max="6" width="23.21875" customWidth="true" style="0"/>
+    <col min="7" max="7" width="14.33203125" customWidth="true" style="0"/>
+    <col min="8" max="8" width="24.33203125" customWidth="true" style="0"/>
+    <col min="9" max="9" width="33.44140625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -3354,58 +3449,58 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -3416,43 +3511,80 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="1" sqref="G2:G3">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="0" showInputMessage="0" showErrorMessage="1" sqref="L2">
       <formula1>"Not Tested,Passed,Failed,On Testing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>"Positive,Negative"</formula1>
-    </dataValidation>
   </dataValidations>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="15.75" defaultColWidth="12.6640625" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="15.75" defaultColWidth="12.6640625" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>